<commit_message>
Finished for the week
</commit_message>
<xml_diff>
--- a/whack_words.xlsx
+++ b/whack_words.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Software\gnarfle\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92D75851-22D7-4529-A46C-2E9843DC4038}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C67C8A91-7C20-43F9-82BD-E6241F3E9605}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{8B52DA7A-9EA2-4E55-9AC4-DC6B68AE6F55}"/>
+    <workbookView xWindow="25668" yWindow="1056" windowWidth="17280" windowHeight="9468" xr2:uid="{8B52DA7A-9EA2-4E55-9AC4-DC6B68AE6F55}"/>
   </bookViews>
   <sheets>
     <sheet name="whackwords" sheetId="2" r:id="rId1"/>
@@ -31,10 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="42">
-  <si>
-    <t>keyword</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
   <si>
     <t>work</t>
   </si>
@@ -157,6 +154,9 @@
   </si>
   <si>
     <t>be a</t>
+  </si>
+  <si>
+    <t>whack_word</t>
   </si>
 </sst>
 </file>
@@ -534,9 +534,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC727665-EF62-45A3-A362-0A80446F2777}">
-  <dimension ref="A1:A44"/>
+  <dimension ref="A1:A42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection sqref="A1:A1048576"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -545,42 +547,42 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.3">
@@ -590,32 +592,32 @@
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>39</v>
+        <v>19</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>30</v>
+        <v>13</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.3">
@@ -625,142 +627,132 @@
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>14</v>
+        <v>36</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>37</v>
+        <v>12</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>13</v>
+        <v>39</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>4</v>
+        <v>24</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>40</v>
+        <v>2</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>25</v>
+        <v>4</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>5</v>
+        <v>28</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>9</v>
+        <v>25</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>22</v>
+        <v>5</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>27</v>
+        <v>10</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>6</v>
+        <v>31</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>10</v>
+        <v>35</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>35</v>
+        <v>0</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>36</v>
+        <v>15</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A43" t="s">
         <v>16</v>
-      </c>
-    </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A44" t="s">
-        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>